<commit_message>
Remove NQ_BEIR_COMPARISON.md and update related files for consistency in BEIR benchmark reporting
- Deleted the `NQ_BEIR_COMPARISON.md` file as it is no longer needed.
- Updated LaTeX and markdown files to include `BM25_TCT` results for better comparison with BEIR benchmarks.
- Adjusted performance metrics in `RESULTS_SUMMARY.md`, `results_table.tex`, and `results.json` to reflect the latest evaluations.
- Updated figures and tables to ensure accurate representation of retrieval performance across different models.
</commit_message>
<xml_diff>
--- a/data/nq/results/paper/results.xlsx
+++ b/data/nq/results/paper/results.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,7 +474,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
@@ -618,30 +618,60 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
+          <t>BM25_TCT</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Late-Int</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.4282</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.4605</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.4748</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.4202</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.6374</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.7497</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
           <t>BM25</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Lexical</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C6" s="2" t="n">
         <v>0.2653</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D6" s="2" t="n">
         <v>0.3044</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E6" s="2" t="n">
         <v>0.3316</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F6" s="2" t="n">
         <v>0.2624</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G6" s="2" t="n">
         <v>0.4737</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H6" s="2" t="n">
         <v>0.7497</v>
       </c>
     </row>
@@ -656,7 +686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,7 +695,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -812,31 +842,64 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
+          <t>BM25_TCT</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Late-Int</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.4605</v>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>ColBERT</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>-12.1%</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>Below</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
           <t>BM25</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Lexical</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C6" s="2" t="n">
         <v>0.3044</v>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>BM25</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E6" s="2" t="n">
         <v>0.329</v>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>-7.5%</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>Below</t>
         </is>

</xml_diff>

<commit_message>
Update model files and results for improved performance metrics and consistency
- Updated various model files (`combmnz.res`, `combsum.res`, `learned_mlp.res`, `learned_multioutput.res`, `learned_per_retriever.res`, `rrf.res`, `wcombmnz_rsd.res`, `wcombsum_rsd.res`, `wrrf_rsd.res`) with new hashes and adjusted sizes for better data management.
- Modified QPP result files (`BM25_MonoT5.res.mmnorm.qpp`, `BM25_TCT.res.mmnorm.qpp`, `BM25.res.mmnorm.qpp`) to reflect updated performance metrics.
- Adjusted LaTeX and markdown files in the results directory to ensure accurate representation of retrieval performance across different models, including updates to `beir_comparison.tex`, `RESULTS_SUMMARY.md`, and `results_table.tex` for consistency in reporting.
- Updated binary files for figures and tables to reflect the latest evaluations.
</commit_message>
<xml_diff>
--- a/data/nq/results/paper/results.xlsx
+++ b/data/nq/results/paper/results.xlsx
@@ -567,22 +567,22 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.49</v>
+        <v>0.4925</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.5153</v>
+        <v>0.518</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.5271</v>
+        <v>0.5303</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.482</v>
+        <v>0.4836</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.6685</v>
+        <v>0.6742</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.7387</v>
+        <v>0.7497</v>
       </c>
     </row>
     <row r="4">
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.5153</v>
+        <v>0.518</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>-3.3%</t>
+          <t>-2.8%</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">

</xml_diff>